<commit_message>
use case, erd diagram
use case, erd diagram
</commit_message>
<xml_diff>
--- a/document/ProductBacklog.xlsx
+++ b/document/ProductBacklog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c85150d796f5087/FPT POLY/DATN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c85150d796f5087/FPT POLY/DATN/Quay-thuoc-99-DATN/document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="224" documentId="8_{5E149F40-FA9F-4B50-A5AF-53C4D25734A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{378BFF72-AC6A-429C-AADF-3A1CB2B7391B}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="8_{5E149F40-FA9F-4B50-A5AF-53C4D25734A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{103E8C87-E556-48E6-B221-9547F2DA4257}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{080109A5-DAE0-4142-809D-4ABD5A4A320E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="144">
   <si>
     <t>ID</t>
   </si>
@@ -525,6 +525,70 @@
   </si>
   <si>
     <t>RQ12</t>
+  </si>
+  <si>
+    <t>+ Nhập trùng số lô, trùng giá, trùng hsd: Cộng dồn với hàng hóa trong kho
++ Khác: Tạo hàng hóa mới</t>
+  </si>
+  <si>
+    <t>Trả hàng theo hóa đơn: chỉ được trả trong vòng 3 ngày kể từ ngày thành công</t>
+  </si>
+  <si>
+    <t>Khi tạo phiếu giao hàng gửi cho giao hàng trạng thái đơn hàng chuyển thành đang giao hàng</t>
+  </si>
+  <si>
+    <t>+ Nhập trùng số lô, trùng giá, trùng hsd: Cộng dồn với hàng hóa trong kho
++ Khác: Tạo hàng hóa mới
++ Nhân viên chỉ được sửa phiếu nhập của mình trong vòng 3 ngày</t>
+  </si>
+  <si>
+    <t>Thống kê
+(trang admin)</t>
+  </si>
+  <si>
+    <t>Tình trạng hàng hóa</t>
+  </si>
+  <si>
+    <t>- Sắp hết hạn 
+- Sắp hết hàng</t>
+  </si>
+  <si>
+    <t>Doanh thu</t>
+  </si>
+  <si>
+    <t>Hiển thị ở trang tổng quan (dashboard)</t>
+  </si>
+  <si>
+    <t>- Hàng hóa bán chạy
+- Khách hàng thân thiết
+- Doanh thu theo ngày
+- Tổng hóa đơn trong ngày</t>
+  </si>
+  <si>
+    <t>Bán hàng</t>
+  </si>
+  <si>
+    <t>Bán hàng
+(trang admin)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Thêm hàng hóa vào giỏ hàng
+- Nhập thông tin khách hàng
+- Nhập số tiền nhận được -&gt; tự tính tiền thối 
+- Nhấn submit -&gt; thêm đơn hàng mới (tình trạng thành công, mua tại cửa hàng: true) -&gt; tích điểm cho khách hàng -&gt; trừ số lượng hàng hóa trong kho </t>
+  </si>
+  <si>
+    <t>Tìm kiếm đơn đã mua</t>
+  </si>
+  <si>
+    <t>- Tìm kiếm đơn hàng (mua tại của hàng) trước đây 
+- Nhấn submit -&gt; load lại thông tin đơn hàng đó (khách hàng, hàng hóa)</t>
+  </si>
+  <si>
+    <t>RQ13</t>
+  </si>
+  <si>
+    <t>RQ14</t>
   </si>
 </sst>
 </file>
@@ -609,21 +673,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -636,8 +691,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -645,8 +700,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -963,817 +1042,917 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EE14F2-21FE-470F-BE03-1F10A983162C}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="22.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="67.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="22.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="67.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" s="8" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" s="5" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="6" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="6" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="75" x14ac:dyDescent="0.3">
       <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" ht="131.25" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" ht="206.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10" ht="187.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
     </row>
     <row r="13" spans="1:10" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:10" ht="187.5" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="8"/>
+      <c r="C18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="6" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="8"/>
+      <c r="C22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
     </row>
     <row r="23" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="8"/>
+      <c r="C23" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
     </row>
     <row r="25" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="6" t="s">
+      <c r="B25" s="8"/>
+      <c r="C25" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
     </row>
     <row r="26" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="6" t="s">
+      <c r="B26" s="8"/>
+      <c r="C26" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="6" t="s">
+      <c r="B27" s="8"/>
+      <c r="C27" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F27" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
     </row>
     <row r="28" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
     </row>
     <row r="29" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="6" t="s">
+      <c r="B29" s="8"/>
+      <c r="C29" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
     </row>
     <row r="30" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A30" s="9"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="6" t="s">
+      <c r="B30" s="8"/>
+      <c r="C30" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="6" t="s">
+      <c r="B31" s="8"/>
+      <c r="C31" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
     </row>
     <row r="32" spans="1:10" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-    </row>
-    <row r="33" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="F32" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="1:10" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="6" t="s">
+      <c r="B33" s="8"/>
+      <c r="C33" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
+      <c r="F33" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
     </row>
     <row r="34" spans="1:10" ht="206.25" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="8"/>
+      <c r="C34" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
+      <c r="F34" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
     </row>
     <row r="35" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="6" t="s">
+      <c r="B35" s="8"/>
+      <c r="C35" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
     </row>
     <row r="36" spans="1:10" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="6" t="s">
+      <c r="B36" s="8"/>
+      <c r="C36" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
     </row>
     <row r="37" spans="1:10" ht="150" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="6" t="s">
+      <c r="B37" s="8"/>
+      <c r="C37" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E37" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
     </row>
     <row r="38" spans="1:10" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="6" t="s">
+      <c r="D38" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
     </row>
     <row r="39" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="6" t="s">
+      <c r="B39" s="8"/>
+      <c r="C39" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E39" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
+      <c r="F39" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="1:10" ht="112.5" x14ac:dyDescent="0.3">
+      <c r="A40" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="F40" s="4"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A41" s="9"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A42" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="75" x14ac:dyDescent="0.3">
+      <c r="A43" s="9"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="F43" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="26">
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="A20:A23"/>
     <mergeCell ref="B32:B37"/>
     <mergeCell ref="A32:A37"/>
     <mergeCell ref="B38:B39"/>
@@ -1782,19 +1961,6 @@
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>